<commit_message>
Inclusión del Analisis del Servicio NPL
</commit_message>
<xml_diff>
--- a/web/plantillas/PlantillaSeguimiento.xlsx
+++ b/web/plantillas/PlantillaSeguimiento.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\seguimientoSeco\web\plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/htdocs/seguimientoSeco/web/plantillas/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EF0B89-92D5-3647-9D13-1EF3ABF77535}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -41,18 +42,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -76,23 +71,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -128,7 +122,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -446,77 +446,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="E2:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.140625" style="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1"/>
-    <col min="5" max="5" width="99.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="55" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.140625" style="1"/>
+    <col min="1" max="2" width="11.1640625" style="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1"/>
+    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="5" t="s">
+    <row r="2" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+    <row r="3" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+    <row r="4" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+    <row r="5" spans="5:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="2"/>
-    </row>
-    <row r="8" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:13" s="3" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E16" s="3"/>
+    <row r="6" spans="5:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>